<commit_message>
Changes to the backlog
</commit_message>
<xml_diff>
--- a/Submission/The backlog.xlsx
+++ b/Submission/The backlog.xlsx
@@ -205,26 +205,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,13 +521,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -560,139 +559,155 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="3">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="3">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="3">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>